<commit_message>
memasukan migration gedung dan ruangan + foreign key
memasukan migration gedung dan ruangan + foreign key

sudah ada create dan update untuk table gedung
</commit_message>
<xml_diff>
--- a/public/Uji_Data/data_uji (2).xlsx
+++ b/public/Uji_Data/data_uji (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mocha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430ADFFC-F0B6-4D28-949C-CFBC35012CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D0F601-88D6-435F-80C2-3AD7A7652252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,66 +16,157 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t>2023-06-30</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+  <si>
+    <t>2023-07-29</t>
   </si>
   <si>
     <t>Aktif</t>
   </si>
   <si>
-    <t>2023-06-28_anak.png</t>
-  </si>
-  <si>
-    <t>2023-06-28_daun.jpg</t>
-  </si>
-  <si>
-    <t>2023-06-10</t>
-  </si>
-  <si>
-    <t>2023-06-28_ads.png</t>
-  </si>
-  <si>
-    <t>2023-06-15</t>
-  </si>
-  <si>
-    <t>Tidak_Aktif</t>
-  </si>
-  <si>
-    <t>2023-06-28_fb.png</t>
-  </si>
-  <si>
-    <t>2023-06-17</t>
-  </si>
-  <si>
-    <t>2023-06-30_feed.png</t>
-  </si>
-  <si>
-    <t>2023-06-30_google.png</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>bbbb</t>
+    <t>2023-07-30</t>
+  </si>
+  <si>
+    <t>2023-07-31</t>
+  </si>
+  <si>
+    <t>UJD230729130533</t>
+  </si>
+  <si>
+    <t>UJD230729130534</t>
+  </si>
+  <si>
+    <t>UJD230729130535</t>
+  </si>
+  <si>
+    <t>UJD230729130536</t>
+  </si>
+  <si>
+    <t>UJD230729130537</t>
+  </si>
+  <si>
+    <t>UJD230729130538</t>
+  </si>
+  <si>
+    <t>UJD230729130539</t>
+  </si>
+  <si>
+    <t>UJD230729130540</t>
+  </si>
+  <si>
+    <t>UJD230729130541</t>
+  </si>
+  <si>
+    <t>UJD230729130542</t>
+  </si>
+  <si>
+    <t>UJD230729130543</t>
+  </si>
+  <si>
+    <t>UJD230729130545</t>
+  </si>
+  <si>
+    <t>UJD230729130546</t>
+  </si>
+  <si>
+    <t>UJD230729130547</t>
+  </si>
+  <si>
+    <t>UJD230729130548</t>
+  </si>
+  <si>
+    <t>Nami</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Vivi</t>
+  </si>
+  <si>
+    <t>Data Uji 1</t>
+  </si>
+  <si>
+    <t>Data Uji 2</t>
+  </si>
+  <si>
+    <t>Data Uji 3</t>
+  </si>
+  <si>
+    <t>Data Uji 4</t>
+  </si>
+  <si>
+    <t>Data Uji 5</t>
+  </si>
+  <si>
+    <t>Data Uji 6</t>
+  </si>
+  <si>
+    <t>Data Uji 7</t>
+  </si>
+  <si>
+    <t>Data Uji 8</t>
+  </si>
+  <si>
+    <t>Data Uji 9</t>
+  </si>
+  <si>
+    <t>Data Uji 10</t>
+  </si>
+  <si>
+    <t>Data Uji 11</t>
+  </si>
+  <si>
+    <t>Data Uji 12</t>
+  </si>
+  <si>
+    <t>Data Uji 13</t>
+  </si>
+  <si>
+    <t>Data Uji 14</t>
+  </si>
+  <si>
+    <t>UJD230729130531</t>
+  </si>
+  <si>
+    <t>UJD230729130544</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,8 +189,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,105 +497,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:H4"/>
+  <dimension ref="B1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1">
+        <v>12345</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>12346</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>12347</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>12348</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>12349</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>12350</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>12351</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>12352</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>12353</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>12354</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
-        <v>22222</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>333333</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>12355</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="D4">
-        <v>44444444</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>12356</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>12357</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>12358</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>12359</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>12360</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>12361</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>